<commit_message>
we add work all test
</commit_message>
<xml_diff>
--- a/src/test/resources/excell/TestData.xlsx
+++ b/src/test/resources/excell/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ercan\eclipse-workspace\datadrivenogren\src\test\resources\excell\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ercan\Documents\workspaces\eclipse-ide-for-java-developers\Bank\src\test\resources\excell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B90E1A-B190-4B37-BA05-32CDEF9ADB96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96112510-FFDF-4939-8E35-8E2DAFB50378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31470" yWindow="1260" windowWidth="26130" windowHeight="11385" xr2:uid="{60B41935-734D-4252-BA8F-CC4473373E63}"/>
+    <workbookView xWindow="31470" yWindow="1260" windowWidth="26130" windowHeight="11385" activeTab="3" xr2:uid="{60B41935-734D-4252-BA8F-CC4473373E63}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCostemerTest" sheetId="2" r:id="rId1"/>
@@ -129,13 +129,13 @@
     <t xml:space="preserve"> Potter</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>can</t>
   </si>
   <si>
     <t>tez</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB76182B-A1B0-4765-A57A-AAAFAD225D7A}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
         <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -574,10 +574,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
         <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
       </c>
       <c r="C5">
         <v>1212</v>
@@ -671,7 +671,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8908EB99-77EC-40DE-AFB4-28957C40F07D}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
excellde N yerine Y yaptik
</commit_message>
<xml_diff>
--- a/src/test/resources/excell/TestData.xlsx
+++ b/src/test/resources/excell/TestData.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ercan\Documents\workspaces\eclipse-ide-for-java-developers\Bank\src\test\resources\excell\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96112510-FFDF-4939-8E35-8E2DAFB50378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{47FD77B4-1EBB-4D3E-878D-E7DF51EDC3BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31470" yWindow="1260" windowWidth="26130" windowHeight="11385" activeTab="3" xr2:uid="{60B41935-734D-4252-BA8F-CC4473373E63}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="26190" windowHeight="16500" activeTab="3" xr2:uid="{60B41935-734D-4252-BA8F-CC4473373E63}"/>
   </bookViews>
   <sheets>
     <sheet name="AddCostemerTest" sheetId="2" r:id="rId1"/>
@@ -19,6 +14,7 @@
     <sheet name="test_suite" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:P21"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -499,7 +495,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>